<commit_message>
tables finales soins et infractions
</commit_message>
<xml_diff>
--- a/Data/EUDA/Tampon/a_la_demande_de_deja_traite.xlsx
+++ b/Data/EUDA/Tampon/a_la_demande_de_deja_traite.xlsx
@@ -441,47 +441,47 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Court / probation / police.deja</t>
+          <t>Court / probation / police.deja.demande</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>General practitioner.deja</t>
+          <t>General practitioner.deja.demande</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Other drug treatment centre.deja</t>
+          <t>Other drug treatment centre.deja.demande</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Other health, medical or social service.deja</t>
+          <t>Other health, medical or social service.deja.demande</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Educational services.deja</t>
+          <t>Educational services.deja.demande</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Self-referral, referral from family, friends, etc.; no other agency/institution involved.deja</t>
+          <t>Self-referral, referral from family, friends, etc.; no other agency/institution involved.deja.demande</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Other.deja</t>
+          <t>Other.deja.demande</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Not known / missing.deja</t>
+          <t>Not known / missing.deja.demande</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Total.deja</t>
+          <t>Total.deja.demande</t>
         </is>
       </c>
     </row>

</xml_diff>